<commit_message>
Working version after Chapter 7
</commit_message>
<xml_diff>
--- a/data/sys-rev/data_extraction_main.xlsx
+++ b/data/sys-rev/data_extraction_main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lm16564_bristol_ac_uk/Documents/Documents/rrr/thesis/data/sys-rev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7846" documentId="8_{3F663B6C-EBE4-49CC-8A72-85CC93C1D1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D578893-2E86-48D3-ACD7-90890C0DF933}"/>
+  <xr:revisionPtr revIDLastSave="7853" documentId="8_{3F663B6C-EBE4-49CC-8A72-85CC93C1D1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B09212E1-7895-4FE0-B512-4A81D391621E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{223BA438-5F2E-4822-A5ED-F5CE1AC6569C}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{223BA438-5F2E-4822-A5ED-F5CE1AC6569C}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="1" r:id="rId1"/>
@@ -6212,8 +6212,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S148"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13196,8 +13196,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AR547"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+    <sheetView tabSelected="1" topLeftCell="A485" workbookViewId="0">
+      <selection activeCell="A548" sqref="A548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44529,11 +44529,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AS547" xr:uid="{06A4228E-D6DA-48FD-8676-3797E7061522}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AR547">
-      <sortCondition ref="C1:C547"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:AS547" xr:uid="{06A4228E-D6DA-48FD-8676-3797E7061522}"/>
   <conditionalFormatting sqref="T12">
     <cfRule type="expression" dxfId="9" priority="5">
       <formula>$C12="D"</formula>
@@ -44584,7 +44580,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>

</xml_diff>